<commit_message>
Update do RAF de janeiro
</commit_message>
<xml_diff>
--- a/Lista.xlsx
+++ b/Lista.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr codeName="EstaPasta_de_trabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IFI\IFI_statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E85D60F-3FB0-4F0D-9A17-5714807D0D99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAF2E48-C775-4843-983B-74F8B15A8C49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6797" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6800" uniqueCount="474">
   <si>
     <t>Nome</t>
   </si>
@@ -1519,6 +1519,12 @@
   <si>
     <t>Sigla</t>
   </si>
+  <si>
+    <t>https://www2.senado.leg.br/bdsf/bitstream/handle/id/583296/RAF48_JAN2021.pdf</t>
+  </si>
+  <si>
+    <t>RAF - Relatório de Acompanhamento Fiscal - Jan/2021</t>
+  </si>
 </sst>
 </file>
 
@@ -1663,9 +1669,16 @@
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -1674,7 +1687,20 @@
       <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -20486,7 +20512,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="Tabela dinâmica2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="Tabela dinâmica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C284" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -21669,8 +21695,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:H116" totalsRowShown="0">
-  <autoFilter ref="A1:H116" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:H117" totalsRowShown="0">
+  <autoFilter ref="A1:H117" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nome"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Categoria"/>
@@ -21682,8 +21708,8 @@
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Nome arquivo">
       <calculatedColumnFormula>MID($D2,60,90)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Data" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{93A6A3EA-E755-4566-AE16-0196F81178A1}" name="Sigla" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Data" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{93A6A3EA-E755-4566-AE16-0196F81178A1}" name="Sigla" dataDxfId="3">
       <calculatedColumnFormula>_xlfn.IFS(Tabela1[[#This Row],[Categoria]]="Estudos Especiais","EE",Tabela1[[#This Row],[Categoria]]="RAF","RAF",Tabela1[[#This Row],[Categoria]]="Nota Técnica","NT",Tabela1[[#This Row],[Categoria]]="Comentários da IFI","CI")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -21965,13 +21991,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H116"/>
+  <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B96" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -25345,9 +25371,41 @@
         <v>RAF</v>
       </c>
     </row>
+    <row r="117" spans="1:8">
+      <c r="A117" s="16" t="s">
+        <v>473</v>
+      </c>
+      <c r="B117" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C117">
+        <v>48</v>
+      </c>
+      <c r="D117" t="s">
+        <v>472</v>
+      </c>
+      <c r="E117" t="str">
+        <f>MID($D117,53,6)</f>
+        <v>583296</v>
+      </c>
+      <c r="F117" t="str">
+        <f>MID($D117,60,90)</f>
+        <v>RAF48_JAN2021.pdf</v>
+      </c>
+      <c r="G117" s="2">
+        <v>44548</v>
+      </c>
+      <c r="H117" s="7" t="str">
+        <f>_xlfn.IFS(Tabela1[[#This Row],[Categoria]]="Estudos Especiais","EE",Tabela1[[#This Row],[Categoria]]="RAF","RAF",Tabela1[[#This Row],[Categoria]]="Nota Técnica","NT",Tabela1[[#This Row],[Categoria]]="Comentários da IFI","CI")</f>
+        <v>RAF</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E247">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E117">
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D68" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>